<commit_message>
host and gallery management
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Excel Files/Club Data/Host Data/Host Data.xlsx
+++ b/cypress/fixtures/Excel Files/Club Data/Host Data/Host Data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Automations\cypress\fixtures\Excel Files\Club Data\Host Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E81CF5-3E2F-40DE-846B-1C6027BE4350}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953DAF72-8CE3-40A6-8A37-6320EEB872EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Moment Club" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="217">
   <si>
     <t>hostName</t>
   </si>
@@ -665,6 +665,18 @@
   </si>
   <si>
     <t>準執行部</t>
+  </si>
+  <si>
+    <t>GalleryImageList</t>
+  </si>
+  <si>
+    <t>["D:/Web Automations/cypress/fixtures/Files/Host Images/profile.jpg","D:/Web Automations/cypress/fixtures/Files/Host Images/host1.jpg","D:/Web Automations/cypress/fixtures/Files/Host Images/host2.jpeg"]</t>
+  </si>
+  <si>
+    <t>D:/Web Automations/cypress/fixtures/Files/Host Images/host1.jpg</t>
+  </si>
+  <si>
+    <t>D:/Web Automations/cypress/fixtures/Files/Host Images/host3.png\</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT11"/>
+  <dimension ref="A1:AU11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="AI17" sqref="AI17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1027,7 @@
     <col min="2" max="2" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1154,14 +1166,23 @@
       <c r="AT1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="C2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" t="s">
+        <v>216</v>
+      </c>
       <c r="E2" t="s">
         <v>211</v>
       </c>
@@ -1192,8 +1213,11 @@
       <c r="Z2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>95</v>
       </c>
@@ -1206,8 +1230,11 @@
       <c r="I3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
@@ -1220,8 +1247,11 @@
       <c r="J4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>99</v>
       </c>
@@ -1241,7 +1271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>101</v>
       </c>
@@ -1258,7 +1288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>103</v>
       </c>
@@ -1269,7 +1299,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>105</v>
       </c>
@@ -1280,7 +1310,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
@@ -1291,7 +1321,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>109</v>
       </c>
@@ -1302,7 +1332,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="11" spans="1:46" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>111</v>
       </c>

</xml_diff>